<commit_message>
It runs, right before adding starting sim weights
</commit_message>
<xml_diff>
--- a/my_code/model_uncert/input/k-means/MH_trans.xlsx
+++ b/my_code/model_uncert/input/k-means/MH_trans.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="7">
   <si>
     <t>Bad MH Type : % transition from bad mental health</t>
   </si>
@@ -137,37 +137,37 @@
         <v>25</v>
       </c>
       <c r="B3">
-        <v>0.87653022511838263</v>
+        <v>0.88466467934928883</v>
       </c>
       <c r="C3">
-        <v>0.12346977488161737</v>
+        <v>0.11533532065071112</v>
       </c>
       <c r="H3">
         <v>25</v>
       </c>
       <c r="I3">
-        <v>0.39822453931279728</v>
+        <v>0.28294071685695732</v>
       </c>
       <c r="J3">
-        <v>0.60177546068720267</v>
+        <v>0.71705928314304279</v>
       </c>
       <c r="N3">
         <v>25</v>
       </c>
       <c r="O3">
-        <v>0.29423497731104881</v>
+        <v>0.28066435675021278</v>
       </c>
       <c r="P3">
-        <v>0.70576502268895114</v>
+        <v>0.71933564324978716</v>
       </c>
       <c r="T3">
         <v>25</v>
       </c>
       <c r="U3">
-        <v>0.78162556294991981</v>
+        <v>0.79651901042181061</v>
       </c>
       <c r="V3">
-        <v>0.21837443705008014</v>
+        <v>0.20348098957818941</v>
       </c>
     </row>
     <row r="4">
@@ -175,37 +175,37 @@
         <v>26</v>
       </c>
       <c r="B4">
-        <v>0.87395627205409987</v>
+        <v>0.87736920924852346</v>
       </c>
       <c r="C4">
-        <v>0.1260437279459001</v>
+        <v>0.12263079075147648</v>
       </c>
       <c r="H4">
         <v>26</v>
       </c>
       <c r="I4">
-        <v>0.37658319050759193</v>
+        <v>0.28557280365269705</v>
       </c>
       <c r="J4">
-        <v>0.62341680949240807</v>
+        <v>0.71442719634730301</v>
       </c>
       <c r="N4">
         <v>26</v>
       </c>
       <c r="O4">
-        <v>0.29252559130432365</v>
+        <v>0.29450713294594377</v>
       </c>
       <c r="P4">
-        <v>0.70747440869567635</v>
+        <v>0.70549286705405612</v>
       </c>
       <c r="T4">
         <v>26</v>
       </c>
       <c r="U4">
-        <v>0.76819313097250685</v>
+        <v>0.77078866768743137</v>
       </c>
       <c r="V4">
-        <v>0.23180686902749317</v>
+        <v>0.22921133231256868</v>
       </c>
     </row>
     <row r="5">
@@ -213,37 +213,37 @@
         <v>27</v>
       </c>
       <c r="B5">
-        <v>0.82499847165683271</v>
+        <v>0.81362127228803982</v>
       </c>
       <c r="C5">
-        <v>0.17500152834316729</v>
+        <v>0.18637872771196023</v>
       </c>
       <c r="H5">
         <v>27</v>
       </c>
       <c r="I5">
-        <v>0.34404688368294079</v>
+        <v>0.34209593386168929</v>
       </c>
       <c r="J5">
-        <v>0.65595311631705921</v>
+        <v>0.65790406613831076</v>
       </c>
       <c r="N5">
         <v>27</v>
       </c>
       <c r="O5">
-        <v>0.25504018553691471</v>
+        <v>0.28285164962531179</v>
       </c>
       <c r="P5">
-        <v>0.74495981446308523</v>
+        <v>0.71714835037468816</v>
       </c>
       <c r="T5">
         <v>27</v>
       </c>
       <c r="U5">
-        <v>0.77949984955494234</v>
+        <v>0.78204173490500573</v>
       </c>
       <c r="V5">
-        <v>0.22050015044505775</v>
+        <v>0.21795826509499433</v>
       </c>
     </row>
     <row r="6">
@@ -251,37 +251,37 @@
         <v>28</v>
       </c>
       <c r="B6">
-        <v>0.8575775352415177</v>
+        <v>0.85748075341796159</v>
       </c>
       <c r="C6">
-        <v>0.14242246475848225</v>
+        <v>0.14251924658203838</v>
       </c>
       <c r="H6">
         <v>28</v>
       </c>
       <c r="I6">
-        <v>0.43625590660398045</v>
+        <v>0.41642000165051024</v>
       </c>
       <c r="J6">
-        <v>0.56374409339601961</v>
+        <v>0.58357999834948981</v>
       </c>
       <c r="N6">
         <v>28</v>
       </c>
       <c r="O6">
-        <v>0.18852078063785588</v>
+        <v>0.17126702670120977</v>
       </c>
       <c r="P6">
-        <v>0.81147921936214407</v>
+        <v>0.82873297329879014</v>
       </c>
       <c r="T6">
         <v>28</v>
       </c>
       <c r="U6">
-        <v>0.76977557193192436</v>
+        <v>0.78437480983222962</v>
       </c>
       <c r="V6">
-        <v>0.23022442806807569</v>
+        <v>0.21562519016777035</v>
       </c>
     </row>
     <row r="7">
@@ -289,37 +289,37 @@
         <v>29</v>
       </c>
       <c r="B7">
-        <v>0.84733845350568238</v>
+        <v>0.85112449895712761</v>
       </c>
       <c r="C7">
-        <v>0.1526615464943176</v>
+        <v>0.14887550104287237</v>
       </c>
       <c r="H7">
         <v>29</v>
       </c>
       <c r="I7">
-        <v>0.38002483683674088</v>
+        <v>0.34561066715694411</v>
       </c>
       <c r="J7">
-        <v>0.61997516316325918</v>
+        <v>0.65438933284305589</v>
       </c>
       <c r="N7">
         <v>29</v>
       </c>
       <c r="O7">
-        <v>0.32144763812362981</v>
+        <v>0.28973670240717253</v>
       </c>
       <c r="P7">
-        <v>0.67855236187637025</v>
+        <v>0.71026329759282747</v>
       </c>
       <c r="T7">
         <v>29</v>
       </c>
       <c r="U7">
-        <v>0.77698228324638985</v>
+        <v>0.78409595404029664</v>
       </c>
       <c r="V7">
-        <v>0.22301771675361015</v>
+        <v>0.21590404595970333</v>
       </c>
     </row>
     <row r="8">
@@ -327,37 +327,37 @@
         <v>30</v>
       </c>
       <c r="B8">
-        <v>0.8638401063512634</v>
+        <v>0.86043904705603658</v>
       </c>
       <c r="C8">
-        <v>0.13615989364873654</v>
+        <v>0.13956095294396342</v>
       </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8">
-        <v>0.40065277807806404</v>
+        <v>0.37643169896275791</v>
       </c>
       <c r="J8">
-        <v>0.5993472219219359</v>
+        <v>0.62356830103724203</v>
       </c>
       <c r="N8">
         <v>30</v>
       </c>
       <c r="O8">
-        <v>0.30478264439729863</v>
+        <v>0.2951895303236402</v>
       </c>
       <c r="P8">
-        <v>0.69521735560270126</v>
+        <v>0.70481046967635974</v>
       </c>
       <c r="T8">
         <v>30</v>
       </c>
       <c r="U8">
-        <v>0.77283425082552049</v>
+        <v>0.77127076031520736</v>
       </c>
       <c r="V8">
-        <v>0.22716574917447951</v>
+        <v>0.22872923968479267</v>
       </c>
     </row>
     <row r="9">
@@ -365,37 +365,37 @@
         <v>31</v>
       </c>
       <c r="B9">
-        <v>0.85775091610851661</v>
+        <v>0.84935724762351317</v>
       </c>
       <c r="C9">
-        <v>0.14224908389148327</v>
+        <v>0.15064275237648683</v>
       </c>
       <c r="H9">
         <v>31</v>
       </c>
       <c r="I9">
-        <v>0.38053732106263938</v>
+        <v>0.3755633005509203</v>
       </c>
       <c r="J9">
-        <v>0.61946267893736062</v>
+        <v>0.62443669944907965</v>
       </c>
       <c r="N9">
         <v>31</v>
       </c>
       <c r="O9">
-        <v>0.17451785035030165</v>
+        <v>0.16924432956856614</v>
       </c>
       <c r="P9">
-        <v>0.82548214964969835</v>
+        <v>0.83075567043143395</v>
       </c>
       <c r="T9">
         <v>31</v>
       </c>
       <c r="U9">
-        <v>0.78478919227477728</v>
+        <v>0.78858334813409392</v>
       </c>
       <c r="V9">
-        <v>0.21521080772522272</v>
+        <v>0.21141665186590602</v>
       </c>
     </row>
     <row r="10">
@@ -403,37 +403,37 @@
         <v>32</v>
       </c>
       <c r="B10">
-        <v>0.85664404815889494</v>
+        <v>0.85380218562147281</v>
       </c>
       <c r="C10">
-        <v>0.14335595184110503</v>
+        <v>0.14619781437852714</v>
       </c>
       <c r="H10">
         <v>32</v>
       </c>
       <c r="I10">
-        <v>0.47108405216680532</v>
+        <v>0.46304882129025937</v>
       </c>
       <c r="J10">
-        <v>0.52891594783319462</v>
+        <v>0.53695117870974063</v>
       </c>
       <c r="N10">
         <v>32</v>
       </c>
       <c r="O10">
-        <v>0.22054273529699958</v>
+        <v>0.2587529667868721</v>
       </c>
       <c r="P10">
-        <v>0.77945726470300047</v>
+        <v>0.74124703321312779</v>
       </c>
       <c r="T10">
         <v>32</v>
       </c>
       <c r="U10">
-        <v>0.76208099822598852</v>
+        <v>0.76136040754145318</v>
       </c>
       <c r="V10">
-        <v>0.23791900177401154</v>
+        <v>0.23863959245854691</v>
       </c>
     </row>
     <row r="11">
@@ -441,37 +441,37 @@
         <v>33</v>
       </c>
       <c r="B11">
-        <v>0.84731293608230529</v>
+        <v>0.84900441070232158</v>
       </c>
       <c r="C11">
-        <v>0.15268706391769471</v>
+        <v>0.15099558929767842</v>
       </c>
       <c r="H11">
         <v>33</v>
       </c>
       <c r="I11">
-        <v>0.35687665535793189</v>
+        <v>0.34945559212551885</v>
       </c>
       <c r="J11">
-        <v>0.64312334464206811</v>
+        <v>0.6505444078744812</v>
       </c>
       <c r="N11">
         <v>33</v>
       </c>
       <c r="O11">
-        <v>0.25181182832838944</v>
+        <v>0.25483904527201667</v>
       </c>
       <c r="P11">
-        <v>0.74818817167161056</v>
+        <v>0.74516095472798327</v>
       </c>
       <c r="T11">
         <v>33</v>
       </c>
       <c r="U11">
-        <v>0.78643712735741933</v>
+        <v>0.79036307747971235</v>
       </c>
       <c r="V11">
-        <v>0.21356287264258073</v>
+        <v>0.20963692252028771</v>
       </c>
     </row>
     <row r="12">
@@ -479,37 +479,37 @@
         <v>34</v>
       </c>
       <c r="B12">
-        <v>0.85587686536535812</v>
+        <v>0.85551413579489832</v>
       </c>
       <c r="C12">
-        <v>0.1441231346346418</v>
+        <v>0.14448586420510168</v>
       </c>
       <c r="H12">
         <v>34</v>
       </c>
       <c r="I12">
-        <v>0.43778042654786675</v>
+        <v>0.43228608712626027</v>
       </c>
       <c r="J12">
-        <v>0.56221957345213314</v>
+        <v>0.56771391287373973</v>
       </c>
       <c r="N12">
         <v>34</v>
       </c>
       <c r="O12">
-        <v>0.27191637289302445</v>
+        <v>0.2945230333888581</v>
       </c>
       <c r="P12">
-        <v>0.72808362710697561</v>
+        <v>0.7054769666111419</v>
       </c>
       <c r="T12">
         <v>34</v>
       </c>
       <c r="U12">
-        <v>0.79012495440429198</v>
+        <v>0.78959893607552867</v>
       </c>
       <c r="V12">
-        <v>0.20987504559570802</v>
+        <v>0.21040106392447142</v>
       </c>
     </row>
     <row r="13">
@@ -517,37 +517,37 @@
         <v>35</v>
       </c>
       <c r="B13">
-        <v>0.86535332589934977</v>
+        <v>0.86482892620618235</v>
       </c>
       <c r="C13">
-        <v>0.1346466741006502</v>
+        <v>0.1351710737938176</v>
       </c>
       <c r="H13">
         <v>35</v>
       </c>
       <c r="I13">
-        <v>0.42461608617338231</v>
+        <v>0.42233561867279323</v>
       </c>
       <c r="J13">
-        <v>0.57538391382661769</v>
+        <v>0.57766438132720666</v>
       </c>
       <c r="N13">
         <v>35</v>
       </c>
       <c r="O13">
-        <v>0.34638150836722725</v>
+        <v>0.36535386513419044</v>
       </c>
       <c r="P13">
-        <v>0.65361849163277275</v>
+        <v>0.63464613486580967</v>
       </c>
       <c r="T13">
         <v>35</v>
       </c>
       <c r="U13">
-        <v>0.78170267123913562</v>
+        <v>0.78155377121398617</v>
       </c>
       <c r="V13">
-        <v>0.21829732876086447</v>
+        <v>0.21844622878601389</v>
       </c>
     </row>
     <row r="14">
@@ -555,37 +555,37 @@
         <v>36</v>
       </c>
       <c r="B14">
-        <v>0.87660198513045695</v>
+        <v>0.87576750286500005</v>
       </c>
       <c r="C14">
-        <v>0.12339801486954309</v>
+        <v>0.12423249713499998</v>
       </c>
       <c r="H14">
         <v>36</v>
       </c>
       <c r="I14">
-        <v>0.43864955384377835</v>
+        <v>0.4358888645196774</v>
       </c>
       <c r="J14">
-        <v>0.56135044615622165</v>
+        <v>0.56411113548032266</v>
       </c>
       <c r="N14">
         <v>36</v>
       </c>
       <c r="O14">
-        <v>0.29035277517603908</v>
+        <v>0.28176724149846383</v>
       </c>
       <c r="P14">
-        <v>0.70964722482396081</v>
+        <v>0.71823275850153623</v>
       </c>
       <c r="T14">
         <v>36</v>
       </c>
       <c r="U14">
-        <v>0.78837615300304353</v>
+        <v>0.79191709824676093</v>
       </c>
       <c r="V14">
-        <v>0.21162384699695655</v>
+        <v>0.20808290175323907</v>
       </c>
     </row>
     <row r="15">
@@ -593,37 +593,37 @@
         <v>37</v>
       </c>
       <c r="B15">
-        <v>0.87026270089853586</v>
+        <v>0.86936503570702106</v>
       </c>
       <c r="C15">
-        <v>0.12973729910146425</v>
+        <v>0.13063496429297888</v>
       </c>
       <c r="H15">
         <v>37</v>
       </c>
       <c r="I15">
-        <v>0.43879533666671566</v>
+        <v>0.43227144241287013</v>
       </c>
       <c r="J15">
-        <v>0.56120466333328434</v>
+        <v>0.56772855758712992</v>
       </c>
       <c r="N15">
         <v>37</v>
       </c>
       <c r="O15">
-        <v>0.24925048343397257</v>
+        <v>0.25030258866945493</v>
       </c>
       <c r="P15">
-        <v>0.75074951656602751</v>
+        <v>0.74969741133054502</v>
       </c>
       <c r="T15">
         <v>37</v>
       </c>
       <c r="U15">
-        <v>0.7858362350851662</v>
+        <v>0.78742242610207702</v>
       </c>
       <c r="V15">
-        <v>0.21416376491483391</v>
+        <v>0.21257757389792309</v>
       </c>
     </row>
     <row r="16">
@@ -631,37 +631,37 @@
         <v>38</v>
       </c>
       <c r="B16">
-        <v>0.86479264499437936</v>
+        <v>0.86396679114337716</v>
       </c>
       <c r="C16">
-        <v>0.1352073550056207</v>
+        <v>0.13603320885662282</v>
       </c>
       <c r="H16">
         <v>38</v>
       </c>
       <c r="I16">
-        <v>0.40261529174044819</v>
+        <v>0.38997726659887505</v>
       </c>
       <c r="J16">
-        <v>0.5973847082595517</v>
+        <v>0.61002273340112501</v>
       </c>
       <c r="N16">
         <v>38</v>
       </c>
       <c r="O16">
-        <v>0.30873324667445884</v>
+        <v>0.31016705903229042</v>
       </c>
       <c r="P16">
-        <v>0.69126675332554111</v>
+        <v>0.68983294096770964</v>
       </c>
       <c r="T16">
         <v>38</v>
       </c>
       <c r="U16">
-        <v>0.78457226335409846</v>
+        <v>0.78550600070625387</v>
       </c>
       <c r="V16">
-        <v>0.21542773664590145</v>
+        <v>0.21449399929374618</v>
       </c>
     </row>
     <row r="17">
@@ -669,37 +669,37 @@
         <v>39</v>
       </c>
       <c r="B17">
-        <v>0.8705430367397794</v>
+        <v>0.86991965195928089</v>
       </c>
       <c r="C17">
-        <v>0.12945696326022063</v>
+        <v>0.13008034804071911</v>
       </c>
       <c r="H17">
         <v>39</v>
       </c>
       <c r="I17">
-        <v>0.41260760984041683</v>
+        <v>0.40535699022606497</v>
       </c>
       <c r="J17">
-        <v>0.58739239015958311</v>
+        <v>0.59464300977393503</v>
       </c>
       <c r="N17">
         <v>39</v>
       </c>
       <c r="O17">
-        <v>0.35062943925537354</v>
+        <v>0.34490888899664252</v>
       </c>
       <c r="P17">
-        <v>0.6493705607446264</v>
+        <v>0.65509111100335737</v>
       </c>
       <c r="T17">
         <v>39</v>
       </c>
       <c r="U17">
-        <v>0.79352701221980604</v>
+        <v>0.79621297940669966</v>
       </c>
       <c r="V17">
-        <v>0.20647298778019391</v>
+        <v>0.20378702059330034</v>
       </c>
     </row>
     <row r="18">
@@ -707,37 +707,37 @@
         <v>40</v>
       </c>
       <c r="B18">
-        <v>0.87439011557987323</v>
+        <v>0.87103717581024853</v>
       </c>
       <c r="C18">
-        <v>0.12560988442012688</v>
+        <v>0.12896282418975155</v>
       </c>
       <c r="H18">
         <v>40</v>
       </c>
       <c r="I18">
-        <v>0.41596195468938324</v>
+        <v>0.41079598342185397</v>
       </c>
       <c r="J18">
-        <v>0.58403804531061687</v>
+        <v>0.58920401657814603</v>
       </c>
       <c r="N18">
         <v>40</v>
       </c>
       <c r="O18">
-        <v>0.29617332634299259</v>
+        <v>0.30462874027741393</v>
       </c>
       <c r="P18">
-        <v>0.70382667365700735</v>
+        <v>0.69537125972258607</v>
       </c>
       <c r="T18">
         <v>40</v>
       </c>
       <c r="U18">
-        <v>0.82303248300873932</v>
+        <v>0.82350287675134326</v>
       </c>
       <c r="V18">
-        <v>0.17696751699126068</v>
+        <v>0.17649712324865671</v>
       </c>
     </row>
     <row r="19">
@@ -745,37 +745,37 @@
         <v>41</v>
       </c>
       <c r="B19">
-        <v>0.86043290398143446</v>
+        <v>0.85251862667503153</v>
       </c>
       <c r="C19">
-        <v>0.13956709601856554</v>
+        <v>0.14748137332496841</v>
       </c>
       <c r="H19">
         <v>41</v>
       </c>
       <c r="I19">
-        <v>0.42277551630385524</v>
+        <v>0.4277284912093024</v>
       </c>
       <c r="J19">
-        <v>0.57722448369614476</v>
+        <v>0.57227150879069766</v>
       </c>
       <c r="N19">
         <v>41</v>
       </c>
       <c r="O19">
-        <v>0.23986285454067924</v>
+        <v>0.24143484344379018</v>
       </c>
       <c r="P19">
-        <v>0.76013714545932087</v>
+        <v>0.75856515655620971</v>
       </c>
       <c r="T19">
         <v>41</v>
       </c>
       <c r="U19">
-        <v>0.82435037676105294</v>
+        <v>0.82611757773972549</v>
       </c>
       <c r="V19">
-        <v>0.17564962323894703</v>
+        <v>0.17388242226027451</v>
       </c>
     </row>
     <row r="20">
@@ -783,37 +783,37 @@
         <v>42</v>
       </c>
       <c r="B20">
-        <v>0.84948991742747637</v>
+        <v>0.84745473200116173</v>
       </c>
       <c r="C20">
-        <v>0.15051008257252368</v>
+        <v>0.15254526799883833</v>
       </c>
       <c r="H20">
         <v>42</v>
       </c>
       <c r="I20">
-        <v>0.38776856331023657</v>
+        <v>0.38542332445020228</v>
       </c>
       <c r="J20">
-        <v>0.61223143668976343</v>
+        <v>0.61457667554979767</v>
       </c>
       <c r="N20">
         <v>42</v>
       </c>
       <c r="O20">
-        <v>0.31229632190970419</v>
+        <v>0.29848831153953681</v>
       </c>
       <c r="P20">
-        <v>0.68770367809029576</v>
+        <v>0.70151168846046319</v>
       </c>
       <c r="T20">
         <v>42</v>
       </c>
       <c r="U20">
-        <v>0.80670108638972349</v>
+        <v>0.8115074319253861</v>
       </c>
       <c r="V20">
-        <v>0.19329891361027654</v>
+        <v>0.18849256807461387</v>
       </c>
     </row>
     <row r="21">
@@ -821,37 +821,37 @@
         <v>43</v>
       </c>
       <c r="B21">
-        <v>0.84706799450425552</v>
+        <v>0.84173998166641695</v>
       </c>
       <c r="C21">
-        <v>0.15293200549574451</v>
+        <v>0.15826001833358308</v>
       </c>
       <c r="H21">
         <v>43</v>
       </c>
       <c r="I21">
-        <v>0.36850038246576622</v>
+        <v>0.370431140520326</v>
       </c>
       <c r="J21">
-        <v>0.63149961753423367</v>
+        <v>0.62956885947967411</v>
       </c>
       <c r="N21">
         <v>43</v>
       </c>
       <c r="O21">
-        <v>0.23884701823088497</v>
+        <v>0.24153642992487354</v>
       </c>
       <c r="P21">
-        <v>0.76115298176911506</v>
+        <v>0.75846357007512644</v>
       </c>
       <c r="T21">
         <v>43</v>
       </c>
       <c r="U21">
-        <v>0.81564232740318277</v>
+        <v>0.81760924097790311</v>
       </c>
       <c r="V21">
-        <v>0.18435767259681726</v>
+        <v>0.18239075902209687</v>
       </c>
     </row>
     <row r="22">
@@ -859,37 +859,37 @@
         <v>44</v>
       </c>
       <c r="B22">
-        <v>0.83593024208217692</v>
+        <v>0.83338032712360177</v>
       </c>
       <c r="C22">
-        <v>0.16406975791782313</v>
+        <v>0.1666196728763982</v>
       </c>
       <c r="H22">
         <v>44</v>
       </c>
       <c r="I22">
-        <v>0.4155020554318184</v>
+        <v>0.41443645737036849</v>
       </c>
       <c r="J22">
-        <v>0.58449794456818172</v>
+        <v>0.5855635426296314</v>
       </c>
       <c r="N22">
         <v>44</v>
       </c>
       <c r="O22">
-        <v>0.3350503611712109</v>
+        <v>0.31984320231921082</v>
       </c>
       <c r="P22">
-        <v>0.6649496388287891</v>
+        <v>0.68015679768078918</v>
       </c>
       <c r="T22">
         <v>44</v>
       </c>
       <c r="U22">
-        <v>0.81416166714340543</v>
+        <v>0.81838977638474775</v>
       </c>
       <c r="V22">
-        <v>0.18583833285659465</v>
+        <v>0.18161022361525214</v>
       </c>
     </row>
     <row r="23">
@@ -897,37 +897,37 @@
         <v>45</v>
       </c>
       <c r="B23">
-        <v>0.85070866375718712</v>
+        <v>0.85071406196243482</v>
       </c>
       <c r="C23">
-        <v>0.14929133624281288</v>
+        <v>0.14928593803756526</v>
       </c>
       <c r="H23">
         <v>45</v>
       </c>
       <c r="I23">
-        <v>0.44412031079816711</v>
+        <v>0.43659462306648722</v>
       </c>
       <c r="J23">
-        <v>0.55587968920183284</v>
+        <v>0.56340537693351267</v>
       </c>
       <c r="N23">
         <v>45</v>
       </c>
       <c r="O23">
-        <v>0.26099126309845583</v>
+        <v>0.2616260054727309</v>
       </c>
       <c r="P23">
-        <v>0.73900873690154412</v>
+        <v>0.73837399452726915</v>
       </c>
       <c r="T23">
         <v>45</v>
       </c>
       <c r="U23">
-        <v>0.81100361344969729</v>
+        <v>0.81148507752246057</v>
       </c>
       <c r="V23">
-        <v>0.18899638655030271</v>
+        <v>0.18851492247753943</v>
       </c>
     </row>
     <row r="24">
@@ -935,37 +935,37 @@
         <v>46</v>
       </c>
       <c r="B24">
-        <v>0.84886742994928488</v>
+        <v>0.84786104611501822</v>
       </c>
       <c r="C24">
-        <v>0.15113257005071518</v>
+        <v>0.15213895388498175</v>
       </c>
       <c r="H24">
         <v>46</v>
       </c>
       <c r="I24">
-        <v>0.45754754486056914</v>
+        <v>0.45026615361240796</v>
       </c>
       <c r="J24">
-        <v>0.54245245513943074</v>
+        <v>0.54973384638759204</v>
       </c>
       <c r="N24">
         <v>46</v>
       </c>
       <c r="O24">
-        <v>0.31971630050134636</v>
+        <v>0.31622279389078484</v>
       </c>
       <c r="P24">
-        <v>0.68028369949865375</v>
+        <v>0.68377720610921511</v>
       </c>
       <c r="T24">
         <v>46</v>
       </c>
       <c r="U24">
-        <v>0.80640921221095985</v>
+        <v>0.80742931883353952</v>
       </c>
       <c r="V24">
-        <v>0.19359078778904007</v>
+        <v>0.19257068116646051</v>
       </c>
     </row>
     <row r="25">
@@ -973,37 +973,37 @@
         <v>47</v>
       </c>
       <c r="B25">
-        <v>0.83944495126579977</v>
+        <v>0.83681466609567623</v>
       </c>
       <c r="C25">
-        <v>0.16055504873420021</v>
+        <v>0.16318533390432391</v>
       </c>
       <c r="H25">
         <v>47</v>
       </c>
       <c r="I25">
-        <v>0.33280742113103734</v>
+        <v>0.33296555140609818</v>
       </c>
       <c r="J25">
-        <v>0.66719257886896277</v>
+        <v>0.66703444859390193</v>
       </c>
       <c r="N25">
         <v>47</v>
       </c>
       <c r="O25">
-        <v>0.29173869110825401</v>
+        <v>0.29520188944460934</v>
       </c>
       <c r="P25">
-        <v>0.70826130889174599</v>
+        <v>0.70479811055539066</v>
       </c>
       <c r="T25">
         <v>47</v>
       </c>
       <c r="U25">
-        <v>0.8145122132383531</v>
+        <v>0.81487413752923954</v>
       </c>
       <c r="V25">
-        <v>0.18548778676164684</v>
+        <v>0.18512586247076049</v>
       </c>
     </row>
     <row r="26">
@@ -1011,37 +1011,37 @@
         <v>48</v>
       </c>
       <c r="B26">
-        <v>0.85297101004791309</v>
+        <v>0.85085052587285304</v>
       </c>
       <c r="C26">
-        <v>0.14702898995208688</v>
+        <v>0.14914947412714707</v>
       </c>
       <c r="H26">
         <v>48</v>
       </c>
       <c r="I26">
-        <v>0.37773759933749596</v>
+        <v>0.37850061334275586</v>
       </c>
       <c r="J26">
-        <v>0.62226240066250393</v>
+        <v>0.62149938665724414</v>
       </c>
       <c r="N26">
         <v>48</v>
       </c>
       <c r="O26">
-        <v>0.2378981645048952</v>
+        <v>0.23924175227565664</v>
       </c>
       <c r="P26">
-        <v>0.7621018354951048</v>
+        <v>0.76075824772434342</v>
       </c>
       <c r="T26">
         <v>48</v>
       </c>
       <c r="U26">
-        <v>0.81169744672528032</v>
+        <v>0.81257832055047863</v>
       </c>
       <c r="V26">
-        <v>0.18830255327471965</v>
+        <v>0.18742167944952143</v>
       </c>
     </row>
     <row r="27">
@@ -1049,37 +1049,37 @@
         <v>49</v>
       </c>
       <c r="B27">
-        <v>0.85523735284625169</v>
+        <v>0.85570179625472997</v>
       </c>
       <c r="C27">
-        <v>0.14476264715374831</v>
+        <v>0.14429820374527003</v>
       </c>
       <c r="H27">
         <v>49</v>
       </c>
       <c r="I27">
-        <v>0.35435746259444695</v>
+        <v>0.35101331048811041</v>
       </c>
       <c r="J27">
-        <v>0.645642537405553</v>
+        <v>0.64898668951188965</v>
       </c>
       <c r="N27">
         <v>49</v>
       </c>
       <c r="O27">
-        <v>0.32149898989496783</v>
+        <v>0.31830636410920365</v>
       </c>
       <c r="P27">
-        <v>0.67850101010503205</v>
+        <v>0.68169363589079635</v>
       </c>
       <c r="T27">
         <v>49</v>
       </c>
       <c r="U27">
-        <v>0.81742900099179538</v>
+        <v>0.81818303062774855</v>
       </c>
       <c r="V27">
-        <v>0.18257099900820464</v>
+        <v>0.18181696937225134</v>
       </c>
     </row>
     <row r="28">
@@ -1087,37 +1087,37 @@
         <v>50</v>
       </c>
       <c r="B28">
-        <v>0.85166773682366104</v>
+        <v>0.84999015139954137</v>
       </c>
       <c r="C28">
-        <v>0.14833226317633888</v>
+        <v>0.1500098486004586</v>
       </c>
       <c r="H28">
         <v>50</v>
       </c>
       <c r="I28">
-        <v>0.41359984262553884</v>
+        <v>0.41119941412223632</v>
       </c>
       <c r="J28">
-        <v>0.58640015737446127</v>
+        <v>0.58880058587776374</v>
       </c>
       <c r="N28">
         <v>50</v>
       </c>
       <c r="O28">
-        <v>0.22249908709768457</v>
+        <v>0.22305875982564477</v>
       </c>
       <c r="P28">
-        <v>0.77750091290231549</v>
+        <v>0.77694124017435529</v>
       </c>
       <c r="T28">
         <v>50</v>
       </c>
       <c r="U28">
-        <v>0.81566785046289181</v>
+        <v>0.81595455982795195</v>
       </c>
       <c r="V28">
-        <v>0.18433214953710816</v>
+        <v>0.18404544017204802</v>
       </c>
     </row>
     <row r="29">
@@ -1125,37 +1125,37 @@
         <v>51</v>
       </c>
       <c r="B29">
-        <v>0.88024643766294264</v>
+        <v>0.87731925768139385</v>
       </c>
       <c r="C29">
-        <v>0.11975356233705745</v>
+        <v>0.12268074231860615</v>
       </c>
       <c r="H29">
         <v>51</v>
       </c>
       <c r="I29">
-        <v>0.39914091855054801</v>
+        <v>0.39881630613492136</v>
       </c>
       <c r="J29">
-        <v>0.60085908144945199</v>
+        <v>0.60118369386507875</v>
       </c>
       <c r="N29">
         <v>51</v>
       </c>
       <c r="O29">
-        <v>0.31196176980399332</v>
+        <v>0.31102130448366516</v>
       </c>
       <c r="P29">
-        <v>0.68803823019600674</v>
+        <v>0.68897869551633484</v>
       </c>
       <c r="T29">
         <v>51</v>
       </c>
       <c r="U29">
-        <v>0.83373935100438223</v>
+        <v>0.83474102011642148</v>
       </c>
       <c r="V29">
-        <v>0.16626064899561771</v>
+        <v>0.16525897988357857</v>
       </c>
     </row>
     <row r="30">
@@ -1163,37 +1163,37 @@
         <v>52</v>
       </c>
       <c r="B30">
-        <v>0.83472390137699326</v>
+        <v>0.83302204753488884</v>
       </c>
       <c r="C30">
-        <v>0.16527609862300671</v>
+        <v>0.16697795246511105</v>
       </c>
       <c r="H30">
         <v>52</v>
       </c>
       <c r="I30">
-        <v>0.3915677642124219</v>
+        <v>0.39151925819073297</v>
       </c>
       <c r="J30">
-        <v>0.6084322357875781</v>
+        <v>0.60848074180926714</v>
       </c>
       <c r="N30">
         <v>52</v>
       </c>
       <c r="O30">
-        <v>0.27061031771008104</v>
+        <v>0.27618088260005541</v>
       </c>
       <c r="P30">
-        <v>0.72938968228991896</v>
+        <v>0.72381911739994464</v>
       </c>
       <c r="T30">
         <v>52</v>
       </c>
       <c r="U30">
-        <v>0.8233256449376718</v>
+        <v>0.82421398067258278</v>
       </c>
       <c r="V30">
-        <v>0.17667435506232815</v>
+        <v>0.17578601932741719</v>
       </c>
     </row>
     <row r="31">
@@ -1201,37 +1201,37 @@
         <v>53</v>
       </c>
       <c r="B31">
-        <v>0.87839797478307635</v>
+        <v>0.87852447685204726</v>
       </c>
       <c r="C31">
-        <v>0.12160202521692363</v>
+        <v>0.12147552314795264</v>
       </c>
       <c r="H31">
         <v>53</v>
       </c>
       <c r="I31">
-        <v>0.40362625438213789</v>
+        <v>0.39994339316981165</v>
       </c>
       <c r="J31">
-        <v>0.59637374561786216</v>
+        <v>0.60005660683018824</v>
       </c>
       <c r="N31">
         <v>53</v>
       </c>
       <c r="O31">
-        <v>0.27215100171922241</v>
+        <v>0.26834091947550043</v>
       </c>
       <c r="P31">
-        <v>0.72784899828077765</v>
+        <v>0.73165908052449957</v>
       </c>
       <c r="T31">
         <v>53</v>
       </c>
       <c r="U31">
-        <v>0.84659782549519835</v>
+        <v>0.84868263839419134</v>
       </c>
       <c r="V31">
-        <v>0.15340217450480167</v>
+        <v>0.15131736160580869</v>
       </c>
     </row>
     <row r="32">
@@ -1239,37 +1239,37 @@
         <v>54</v>
       </c>
       <c r="B32">
-        <v>0.87950821855950212</v>
+        <v>0.8774398655875234</v>
       </c>
       <c r="C32">
-        <v>0.12049178144049791</v>
+        <v>0.12256013441247655</v>
       </c>
       <c r="H32">
         <v>54</v>
       </c>
       <c r="I32">
-        <v>0.40670359745864654</v>
+        <v>0.40447412763669638</v>
       </c>
       <c r="J32">
-        <v>0.59329640254135352</v>
+        <v>0.59552587236330357</v>
       </c>
       <c r="N32">
         <v>54</v>
       </c>
       <c r="O32">
-        <v>0.2848790572551439</v>
+        <v>0.2871628374223304</v>
       </c>
       <c r="P32">
-        <v>0.71512094274485616</v>
+        <v>0.7128371625776696</v>
       </c>
       <c r="T32">
         <v>54</v>
       </c>
       <c r="U32">
-        <v>0.82439613788670441</v>
+        <v>0.82460786379916284</v>
       </c>
       <c r="V32">
-        <v>0.17560386211329562</v>
+        <v>0.17539213620083707</v>
       </c>
     </row>
     <row r="33">
@@ -1277,37 +1277,37 @@
         <v>55</v>
       </c>
       <c r="B33">
-        <v>0.85739533018574088</v>
+        <v>0.85594660958918956</v>
       </c>
       <c r="C33">
-        <v>0.14260466981425901</v>
+        <v>0.14405339041081039</v>
       </c>
       <c r="H33">
         <v>55</v>
       </c>
       <c r="I33">
-        <v>0.39169695956001266</v>
+        <v>0.39086526484211453</v>
       </c>
       <c r="J33">
-        <v>0.60830304043998729</v>
+        <v>0.60913473515788541</v>
       </c>
       <c r="N33">
         <v>55</v>
       </c>
       <c r="O33">
-        <v>0.32422422722840444</v>
+        <v>0.33481334881015684</v>
       </c>
       <c r="P33">
-        <v>0.67577577277159562</v>
+        <v>0.6651866511898431</v>
       </c>
       <c r="T33">
         <v>55</v>
       </c>
       <c r="U33">
-        <v>0.83104558981707211</v>
+        <v>0.83117695129286806</v>
       </c>
       <c r="V33">
-        <v>0.16895441018292792</v>
+        <v>0.16882304870713194</v>
       </c>
     </row>
     <row r="34">
@@ -1315,37 +1315,37 @@
         <v>56</v>
       </c>
       <c r="B34">
-        <v>0.87228754292915844</v>
+        <v>0.87076065137593339</v>
       </c>
       <c r="C34">
-        <v>0.12771245707084158</v>
+        <v>0.12923934862406664</v>
       </c>
       <c r="H34">
         <v>56</v>
       </c>
       <c r="I34">
-        <v>0.36601610997605316</v>
+        <v>0.36584355033041976</v>
       </c>
       <c r="J34">
-        <v>0.63398389002394673</v>
+        <v>0.63415644966958029</v>
       </c>
       <c r="N34">
         <v>56</v>
       </c>
       <c r="O34">
-        <v>0.32263686244651468</v>
+        <v>0.32585231095707251</v>
       </c>
       <c r="P34">
-        <v>0.67736313755348532</v>
+        <v>0.67414768904292743</v>
       </c>
       <c r="T34">
         <v>56</v>
       </c>
       <c r="U34">
-        <v>0.83641938750793388</v>
+        <v>0.83692953995059483</v>
       </c>
       <c r="V34">
-        <v>0.1635806124920661</v>
+        <v>0.16307046004940512</v>
       </c>
     </row>
     <row r="35">
@@ -1353,37 +1353,37 @@
         <v>57</v>
       </c>
       <c r="B35">
-        <v>0.86106173457017532</v>
+        <v>0.85867237306659983</v>
       </c>
       <c r="C35">
-        <v>0.13893826542982471</v>
+        <v>0.14132762693340015</v>
       </c>
       <c r="H35">
         <v>57</v>
       </c>
       <c r="I35">
-        <v>0.40828431423230471</v>
+        <v>0.40962590896991363</v>
       </c>
       <c r="J35">
-        <v>0.59171568576769529</v>
+        <v>0.59037409103008642</v>
       </c>
       <c r="N35">
         <v>57</v>
       </c>
       <c r="O35">
-        <v>0.2505818437207758</v>
+        <v>0.25020117470944947</v>
       </c>
       <c r="P35">
-        <v>0.74941815627922415</v>
+        <v>0.74979882529055042</v>
       </c>
       <c r="T35">
         <v>57</v>
       </c>
       <c r="U35">
-        <v>0.86042422340538949</v>
+        <v>0.86179232318717602</v>
       </c>
       <c r="V35">
-        <v>0.13957577659461054</v>
+        <v>0.13820767681282409</v>
       </c>
     </row>
     <row r="36">
@@ -1391,37 +1391,37 @@
         <v>58</v>
       </c>
       <c r="B36">
-        <v>0.86212724333460455</v>
+        <v>0.86073444991234216</v>
       </c>
       <c r="C36">
-        <v>0.13787275666539547</v>
+        <v>0.13926555008765795</v>
       </c>
       <c r="H36">
         <v>58</v>
       </c>
       <c r="I36">
-        <v>0.37093786181075</v>
+        <v>0.36694998632215536</v>
       </c>
       <c r="J36">
-        <v>0.62906213818924994</v>
+        <v>0.63305001367784464</v>
       </c>
       <c r="N36">
         <v>58</v>
       </c>
       <c r="O36">
-        <v>0.26729505686754013</v>
+        <v>0.27483081400131459</v>
       </c>
       <c r="P36">
-        <v>0.73270494313245993</v>
+        <v>0.72516918599868541</v>
       </c>
       <c r="T36">
         <v>58</v>
       </c>
       <c r="U36">
-        <v>0.84602591911032954</v>
+        <v>0.8468590710396684</v>
       </c>
       <c r="V36">
-        <v>0.15397408088967052</v>
+        <v>0.1531409289603316</v>
       </c>
     </row>
     <row r="37">
@@ -1429,37 +1429,37 @@
         <v>59</v>
       </c>
       <c r="B37">
-        <v>0.86003785623028572</v>
+        <v>0.8608197472428587</v>
       </c>
       <c r="C37">
-        <v>0.13996214376971425</v>
+        <v>0.13918025275714138</v>
       </c>
       <c r="H37">
         <v>59</v>
       </c>
       <c r="I37">
-        <v>0.4037748331612025</v>
+        <v>0.39279460874841576</v>
       </c>
       <c r="J37">
-        <v>0.59622516683879756</v>
+        <v>0.60720539125158424</v>
       </c>
       <c r="N37">
         <v>59</v>
       </c>
       <c r="O37">
-        <v>0.28954711466858724</v>
+        <v>0.28065346647114714</v>
       </c>
       <c r="P37">
-        <v>0.71045288533141282</v>
+        <v>0.71934653352885281</v>
       </c>
       <c r="T37">
         <v>59</v>
       </c>
       <c r="U37">
-        <v>0.83322713978533003</v>
+        <v>0.83497336875848593</v>
       </c>
       <c r="V37">
-        <v>0.16677286021467005</v>
+        <v>0.16502663124151409</v>
       </c>
     </row>
     <row r="38">
@@ -1467,37 +1467,37 @@
         <v>60</v>
       </c>
       <c r="B38">
-        <v>0.85322248454475302</v>
+        <v>0.85380169452997501</v>
       </c>
       <c r="C38">
-        <v>0.14677751545524703</v>
+        <v>0.14619830547002499</v>
       </c>
       <c r="H38">
         <v>60</v>
       </c>
       <c r="I38">
-        <v>0.40949481249937136</v>
+        <v>0.3996459264609265</v>
       </c>
       <c r="J38">
-        <v>0.59050518750062864</v>
+        <v>0.60035407353907355</v>
       </c>
       <c r="N38">
         <v>60</v>
       </c>
       <c r="O38">
-        <v>0.3062447429428139</v>
+        <v>0.3044450770926399</v>
       </c>
       <c r="P38">
-        <v>0.69375525705718621</v>
+        <v>0.6955549229073601</v>
       </c>
       <c r="T38">
         <v>60</v>
       </c>
       <c r="U38">
-        <v>0.85583183635213922</v>
+        <v>0.85689133578203269</v>
       </c>
       <c r="V38">
-        <v>0.14416816364786075</v>
+        <v>0.14310866421796722</v>
       </c>
     </row>
     <row r="39">
@@ -1505,37 +1505,37 @@
         <v>61</v>
       </c>
       <c r="B39">
-        <v>0.84998765135052923</v>
+        <v>0.84697423958718754</v>
       </c>
       <c r="C39">
-        <v>0.1500123486494708</v>
+        <v>0.15302576041281249</v>
       </c>
       <c r="H39">
         <v>61</v>
       </c>
       <c r="I39">
-        <v>0.38896417708499653</v>
+        <v>0.38356126850229377</v>
       </c>
       <c r="J39">
-        <v>0.61103582291500336</v>
+        <v>0.61643873149770623</v>
       </c>
       <c r="N39">
         <v>61</v>
       </c>
       <c r="O39">
-        <v>0.30332949025461164</v>
+        <v>0.3074239501137046</v>
       </c>
       <c r="P39">
-        <v>0.69667050974538836</v>
+        <v>0.6925760498862954</v>
       </c>
       <c r="T39">
         <v>61</v>
       </c>
       <c r="U39">
-        <v>0.85467298573152961</v>
+        <v>0.8546174807404241</v>
       </c>
       <c r="V39">
-        <v>0.14532701426847039</v>
+        <v>0.14538251925957579</v>
       </c>
     </row>
     <row r="40">
@@ -1543,37 +1543,37 @@
         <v>62</v>
       </c>
       <c r="B40">
-        <v>0.87181059798245863</v>
+        <v>0.86824649468508641</v>
       </c>
       <c r="C40">
-        <v>0.12818940201754137</v>
+        <v>0.13175350531491359</v>
       </c>
       <c r="H40">
         <v>62</v>
       </c>
       <c r="I40">
-        <v>0.38308859914801358</v>
+        <v>0.38222523153136279</v>
       </c>
       <c r="J40">
-        <v>0.61691140085198648</v>
+        <v>0.61777476846863721</v>
       </c>
       <c r="N40">
         <v>62</v>
       </c>
       <c r="O40">
-        <v>0.29719406615830629</v>
+        <v>0.29579477390528586</v>
       </c>
       <c r="P40">
-        <v>0.70280593384169376</v>
+        <v>0.70420522609471414</v>
       </c>
       <c r="T40">
         <v>62</v>
       </c>
       <c r="U40">
-        <v>0.86691667206327561</v>
+        <v>0.86813907679342694</v>
       </c>
       <c r="V40">
-        <v>0.13308332793672428</v>
+        <v>0.13186092320657303</v>
       </c>
     </row>
     <row r="41">
@@ -1581,37 +1581,37 @@
         <v>63</v>
       </c>
       <c r="B41">
-        <v>0.88656404554817192</v>
+        <v>0.88721432607740236</v>
       </c>
       <c r="C41">
-        <v>0.11343595445182811</v>
+        <v>0.11278567392259761</v>
       </c>
       <c r="H41">
         <v>63</v>
       </c>
       <c r="I41">
-        <v>0.36656705881430607</v>
+        <v>0.36154185703659253</v>
       </c>
       <c r="J41">
-        <v>0.63343294118569393</v>
+        <v>0.63845814296340753</v>
       </c>
       <c r="N41">
         <v>63</v>
       </c>
       <c r="O41">
-        <v>0.19932539841315877</v>
+        <v>0.19949765550518136</v>
       </c>
       <c r="P41">
-        <v>0.80067460158684112</v>
+        <v>0.80050234449481861</v>
       </c>
       <c r="T41">
         <v>63</v>
       </c>
       <c r="U41">
-        <v>0.86706949290065805</v>
+        <v>0.86861544233472432</v>
       </c>
       <c r="V41">
-        <v>0.13293050709934195</v>
+        <v>0.13138455766527565</v>
       </c>
     </row>
     <row r="42">
@@ -1619,37 +1619,37 @@
         <v>64</v>
       </c>
       <c r="B42">
-        <v>0.81927843129139422</v>
+        <v>0.81524110334207134</v>
       </c>
       <c r="C42">
-        <v>0.18072156870860587</v>
+        <v>0.18475889665792861</v>
       </c>
       <c r="H42">
         <v>64</v>
       </c>
       <c r="I42">
-        <v>0.35214059788009816</v>
+        <v>0.3505669093819469</v>
       </c>
       <c r="J42">
-        <v>0.64785940211990189</v>
+        <v>0.6494330906180531</v>
       </c>
       <c r="N42">
         <v>64</v>
       </c>
       <c r="O42">
-        <v>0.35849468263281997</v>
+        <v>0.35446338382822512</v>
       </c>
       <c r="P42">
-        <v>0.64150531736717997</v>
+        <v>0.64553661617177482</v>
       </c>
       <c r="T42">
         <v>64</v>
       </c>
       <c r="U42">
-        <v>0.87387547208295002</v>
+        <v>0.87427900629162458</v>
       </c>
       <c r="V42">
-        <v>0.12612452791704998</v>
+        <v>0.12572099370837533</v>
       </c>
     </row>
     <row r="43">
@@ -1657,37 +1657,37 @@
         <v>65</v>
       </c>
       <c r="B43">
-        <v>0.86843454229518435</v>
+        <v>0.8664820627848584</v>
       </c>
       <c r="C43">
-        <v>0.13156545770481567</v>
+        <v>0.13351793721514166</v>
       </c>
       <c r="H43">
         <v>65</v>
       </c>
       <c r="I43">
-        <v>0.29884290842599182</v>
+        <v>0.2959587095099579</v>
       </c>
       <c r="J43">
-        <v>0.70115709157400807</v>
+        <v>0.70404129049004216</v>
       </c>
       <c r="N43">
         <v>65</v>
       </c>
       <c r="O43">
-        <v>0.30739433126140997</v>
+        <v>0.32419259902758196</v>
       </c>
       <c r="P43">
-        <v>0.69260566873858997</v>
+        <v>0.67580740097241809</v>
       </c>
       <c r="T43">
         <v>65</v>
       </c>
       <c r="U43">
-        <v>0.875890643360143</v>
+        <v>0.87571299569143413</v>
       </c>
       <c r="V43">
-        <v>0.12410935663985706</v>
+        <v>0.12428700430856596</v>
       </c>
     </row>
     <row r="44">
@@ -1695,37 +1695,37 @@
         <v>66</v>
       </c>
       <c r="B44">
-        <v>0.86583262153772211</v>
+        <v>0.86380528640338394</v>
       </c>
       <c r="C44">
-        <v>0.13416737846227789</v>
+        <v>0.13619471359661606</v>
       </c>
       <c r="H44">
         <v>66</v>
       </c>
       <c r="I44">
-        <v>0.3778557119593528</v>
+        <v>0.37713792752556535</v>
       </c>
       <c r="J44">
-        <v>0.62214428804064714</v>
+        <v>0.6228620724744347</v>
       </c>
       <c r="N44">
         <v>66</v>
       </c>
       <c r="O44">
-        <v>0.25119319271276486</v>
+        <v>0.27378008391074438</v>
       </c>
       <c r="P44">
-        <v>0.74880680728723503</v>
+        <v>0.72621991608925562</v>
       </c>
       <c r="T44">
         <v>66</v>
       </c>
       <c r="U44">
-        <v>0.88049362070908777</v>
+        <v>0.88106113198736313</v>
       </c>
       <c r="V44">
-        <v>0.11950637929091235</v>
+        <v>0.11893886801263687</v>
       </c>
     </row>
     <row r="45">
@@ -1733,37 +1733,37 @@
         <v>67</v>
       </c>
       <c r="B45">
-        <v>0.86237824493402793</v>
+        <v>0.85610692584564596</v>
       </c>
       <c r="C45">
-        <v>0.13762175506597221</v>
+        <v>0.14389307415435401</v>
       </c>
       <c r="H45">
         <v>67</v>
       </c>
       <c r="I45">
-        <v>0.34590733315213584</v>
+        <v>0.34865320792703519</v>
       </c>
       <c r="J45">
-        <v>0.65409266684786416</v>
+        <v>0.65134679207296486</v>
       </c>
       <c r="N45">
         <v>67</v>
       </c>
       <c r="O45">
-        <v>0.31728046678266197</v>
+        <v>0.32802859281568958</v>
       </c>
       <c r="P45">
-        <v>0.68271953321733814</v>
+        <v>0.67197140718431037</v>
       </c>
       <c r="T45">
         <v>67</v>
       </c>
       <c r="U45">
-        <v>0.87497567331765969</v>
+        <v>0.87584330995972715</v>
       </c>
       <c r="V45">
-        <v>0.12502432668234031</v>
+        <v>0.12415669004027284</v>
       </c>
     </row>
     <row r="46">
@@ -1771,37 +1771,37 @@
         <v>68</v>
       </c>
       <c r="B46">
-        <v>0.85019651152380527</v>
+        <v>0.84060426519113729</v>
       </c>
       <c r="C46">
-        <v>0.14980348847619479</v>
+        <v>0.1593957348088626</v>
       </c>
       <c r="H46">
         <v>68</v>
       </c>
       <c r="I46">
-        <v>0.30808878518837662</v>
+        <v>0.31238915686589225</v>
       </c>
       <c r="J46">
-        <v>0.69191121481162332</v>
+        <v>0.6876108431341077</v>
       </c>
       <c r="N46">
         <v>68</v>
       </c>
       <c r="O46">
-        <v>0.24258895450369605</v>
+        <v>0.27024708828160093</v>
       </c>
       <c r="P46">
-        <v>0.757411045496304</v>
+        <v>0.72975291171839907</v>
       </c>
       <c r="T46">
         <v>68</v>
       </c>
       <c r="U46">
-        <v>0.87532230895221985</v>
+        <v>0.87558733382870446</v>
       </c>
       <c r="V46">
-        <v>0.12467769104778005</v>
+        <v>0.12441266617129559</v>
       </c>
     </row>
     <row r="47">
@@ -1809,37 +1809,37 @@
         <v>69</v>
       </c>
       <c r="B47">
-        <v>0.87277653684604195</v>
+        <v>0.8781763753890508</v>
       </c>
       <c r="C47">
-        <v>0.12722346315395808</v>
+        <v>0.12182362461094921</v>
       </c>
       <c r="H47">
         <v>69</v>
       </c>
       <c r="I47">
-        <v>0.3609802330353315</v>
+        <v>0.35539191682602139</v>
       </c>
       <c r="J47">
-        <v>0.63901976696466845</v>
+        <v>0.64460808317397855</v>
       </c>
       <c r="N47">
         <v>69</v>
       </c>
       <c r="O47">
-        <v>0.26318745950578426</v>
+        <v>0.22039193571048152</v>
       </c>
       <c r="P47">
-        <v>0.73681254049421585</v>
+        <v>0.77960806428951834</v>
       </c>
       <c r="T47">
         <v>69</v>
       </c>
       <c r="U47">
-        <v>0.85116386815479717</v>
+        <v>0.85454490452867005</v>
       </c>
       <c r="V47">
-        <v>0.14883613184520289</v>
+        <v>0.14545509547132993</v>
       </c>
     </row>
     <row r="48">
@@ -1847,37 +1847,37 @@
         <v>70</v>
       </c>
       <c r="B48">
-        <v>0.85142688240008457</v>
+        <v>0.85582977158332241</v>
       </c>
       <c r="C48">
-        <v>0.14857311759991537</v>
+        <v>0.14417022841667756</v>
       </c>
       <c r="H48">
         <v>70</v>
       </c>
       <c r="I48">
-        <v>0.33288221829899672</v>
+        <v>0.31158191521689815</v>
       </c>
       <c r="J48">
-        <v>0.66711778170100322</v>
+        <v>0.68841808478310185</v>
       </c>
       <c r="N48">
         <v>70</v>
       </c>
       <c r="O48">
-        <v>0.18658803494375623</v>
+        <v>0.17438742418274303</v>
       </c>
       <c r="P48">
-        <v>0.81341196505624369</v>
+        <v>0.825612575817257</v>
       </c>
       <c r="T48">
         <v>70</v>
       </c>
       <c r="U48">
-        <v>0.86657568385077932</v>
+        <v>0.8650964440040888</v>
       </c>
       <c r="V48">
-        <v>0.13342431614922062</v>
+        <v>0.1349035559959112</v>
       </c>
     </row>
     <row r="49">
@@ -1885,37 +1885,37 @@
         <v>71</v>
       </c>
       <c r="B49">
-        <v>0.84909152218767625</v>
+        <v>0.84916458700636865</v>
       </c>
       <c r="C49">
-        <v>0.15090847781232375</v>
+        <v>0.15083541299363135</v>
       </c>
       <c r="H49">
         <v>71</v>
       </c>
       <c r="I49">
-        <v>0.37066614956492144</v>
+        <v>0.35695422320301773</v>
       </c>
       <c r="J49">
-        <v>0.62933385043507861</v>
+        <v>0.64304577679698227</v>
       </c>
       <c r="N49">
         <v>71</v>
       </c>
       <c r="O49">
-        <v>0.32462452159561617</v>
+        <v>0.35082993025869652</v>
       </c>
       <c r="P49">
-        <v>0.67537547840438394</v>
+        <v>0.64917006974130353</v>
       </c>
       <c r="T49">
         <v>71</v>
       </c>
       <c r="U49">
-        <v>0.85819412173868292</v>
+        <v>0.85557260741794816</v>
       </c>
       <c r="V49">
-        <v>0.14180587826131705</v>
+        <v>0.14442739258205184</v>
       </c>
     </row>
     <row r="50">
@@ -1923,37 +1923,37 @@
         <v>72</v>
       </c>
       <c r="B50">
-        <v>0.82202584326514605</v>
+        <v>0.82860428201800052</v>
       </c>
       <c r="C50">
-        <v>0.17797415673485401</v>
+        <v>0.17139571798199948</v>
       </c>
       <c r="H50">
         <v>72</v>
       </c>
       <c r="I50">
-        <v>0.35371390762291449</v>
+        <v>0.33559892564907556</v>
       </c>
       <c r="J50">
-        <v>0.64628609237708545</v>
+        <v>0.66440107435092455</v>
       </c>
       <c r="N50">
         <v>72</v>
       </c>
       <c r="O50">
-        <v>0.2240481153856474</v>
+        <v>0.19583139033829455</v>
       </c>
       <c r="P50">
-        <v>0.77595188461435272</v>
+        <v>0.80416860966170545</v>
       </c>
       <c r="T50">
         <v>72</v>
       </c>
       <c r="U50">
-        <v>0.84570516614238223</v>
+        <v>0.84819492168434008</v>
       </c>
       <c r="V50">
-        <v>0.15429483385761777</v>
+        <v>0.15180507831566004</v>
       </c>
     </row>
     <row r="51">
@@ -1961,37 +1961,37 @@
         <v>73</v>
       </c>
       <c r="B51">
-        <v>0.84214408208228497</v>
+        <v>0.83840103459113302</v>
       </c>
       <c r="C51">
-        <v>0.15785591791771492</v>
+        <v>0.16159896540886701</v>
       </c>
       <c r="H51">
         <v>73</v>
       </c>
       <c r="I51">
-        <v>0.36986695326574676</v>
+        <v>0.34675354309763967</v>
       </c>
       <c r="J51">
-        <v>0.6301330467342533</v>
+        <v>0.65324645690236038</v>
       </c>
       <c r="N51">
         <v>73</v>
       </c>
       <c r="O51">
-        <v>0.23737714772538887</v>
+        <v>0.19589626394720713</v>
       </c>
       <c r="P51">
-        <v>0.76262285227461113</v>
+        <v>0.80410373605279295</v>
       </c>
       <c r="T51">
         <v>73</v>
       </c>
       <c r="U51">
-        <v>0.84497193883954302</v>
+        <v>0.84681743969436274</v>
       </c>
       <c r="V51">
-        <v>0.15502806116045689</v>
+        <v>0.15318256030563734</v>
       </c>
     </row>
     <row r="52">
@@ -1999,37 +1999,37 @@
         <v>74</v>
       </c>
       <c r="B52">
-        <v>0.82984200899908267</v>
+        <v>0.82723294798766234</v>
       </c>
       <c r="C52">
-        <v>0.17015799100091736</v>
+        <v>0.17276705201233769</v>
       </c>
       <c r="H52">
         <v>74</v>
       </c>
       <c r="I52">
-        <v>0.37699773449049984</v>
+        <v>0.34476563695067874</v>
       </c>
       <c r="J52">
-        <v>0.62300226550950011</v>
+        <v>0.65523436304932126</v>
       </c>
       <c r="N52">
         <v>74</v>
       </c>
       <c r="O52">
-        <v>0.22768528535227739</v>
+        <v>0.18388493059490224</v>
       </c>
       <c r="P52">
-        <v>0.77231471464772261</v>
+        <v>0.81611506940509781</v>
       </c>
       <c r="T52">
         <v>74</v>
       </c>
       <c r="U52">
-        <v>0.86969317298901772</v>
+        <v>0.86690192973648927</v>
       </c>
       <c r="V52">
-        <v>0.13030682701098231</v>
+        <v>0.13309807026351075</v>
       </c>
     </row>
     <row r="53">
@@ -2037,37 +2037,37 @@
         <v>75</v>
       </c>
       <c r="B53">
-        <v>0.85452926028237308</v>
+        <v>0.72715818648260344</v>
       </c>
       <c r="C53">
-        <v>0.14547073971762686</v>
+        <v>0.27284181351739656</v>
       </c>
       <c r="H53">
         <v>75</v>
       </c>
       <c r="I53">
-        <v>0.38660759586311116</v>
+        <v>0.47587694964748178</v>
       </c>
       <c r="J53">
-        <v>0.61339240413688889</v>
+        <v>0.52412305035251827</v>
       </c>
       <c r="N53">
         <v>75</v>
       </c>
       <c r="O53">
-        <v>0.42502006954003352</v>
+        <v>0.62485663979459027</v>
       </c>
       <c r="P53">
-        <v>0.57497993045996654</v>
+        <v>0.37514336020540984</v>
       </c>
       <c r="T53">
         <v>75</v>
       </c>
       <c r="U53">
-        <v>0.83576238678008974</v>
+        <v>0.82328960795449868</v>
       </c>
       <c r="V53">
-        <v>0.16423761321991023</v>
+        <v>0.17671039204550135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>